<commit_message>
some paths are corrected
</commit_message>
<xml_diff>
--- a/docs/STAFF-DATA/001.xlsx
+++ b/docs/STAFF-DATA/001.xlsx
@@ -52,7 +52,7 @@
     <t>Professor &amp; Head</t>
   </si>
   <si>
-    <t>/static/images/profile_photos/001/VEC-001-01-077.jpg</t>
+    <t>/static/images/profile_photos/001/VEC-001-01-077.webp</t>
   </si>
   <si>
     <t>https://scholar.google.co.in/citations?view_op=list_works&amp;hl=en&amp;authuser=2&amp;hl=en&amp;user=KfwgAmoAAAAJ&amp;sortby=pubdate&amp;authuser=2</t>
@@ -82,7 +82,7 @@
     <t>Assistant Professor</t>
   </si>
   <si>
-    <t>/static/images/profile_photos/001/VEC-001-04-080.jpg</t>
+    <t>/static/images/profile_photos/001/VEC-001-04-080.webp</t>
   </si>
   <si>
     <t>https://scholar.google.co.in/citations?view_op=new_articles&amp;hl=en&amp;imq=prema%40velammal.edu.in&amp;nuan-1=premanila21%40gmail.com&amp;authuser=1#</t>
@@ -97,7 +97,7 @@
     <t>RajaSuganya</t>
   </si>
   <si>
-    <t>/static/images/profile_photos/001/VEC-001-04-085.jpg</t>
+    <t>/static/images/profile_photos/001/VEC-001-04-085.webp</t>
   </si>
   <si>
     <t>https://scholar.google.com/citations?hl=en&amp;user=VyAc3CUAAAAJ</t>
@@ -121,7 +121,7 @@
     <t>KAVITHA</t>
   </si>
   <si>
-    <t>/static/images/profile_photos/001/VEC-001-04-075.jpg</t>
+    <t>/static/images/profile_photos/001/VEC-001-04-075.webp</t>
   </si>
   <si>
     <t>https://scholar.google.com/citations?view_op=new_articles&amp;hl=en&amp;imq=Kavitha+Ravi&amp;authuser=1#</t>
@@ -139,7 +139,7 @@
     <t>Hannah Rose Esther</t>
   </si>
   <si>
-    <t>/static/images/profile_photos/001/VEC-001-04-060.jpg</t>
+    <t>/static/images/profile_photos/001/VEC-001-04-060.webp</t>
   </si>
   <si>
     <t>https://scholar.google.com/citations?view_op=list_works&amp;hl=en&amp;user=97zWPAYAAAAJ</t>
@@ -166,7 +166,7 @@
     <t xml:space="preserve">Vijayalakshmi </t>
   </si>
   <si>
-    <t>/static/images/profile_photos/001/VEC-001-04-086.jpg</t>
+    <t>/static/images/profile_photos/001/VEC-001-04-086.webp</t>
   </si>
   <si>
     <t>Nil</t>
@@ -184,7 +184,7 @@
     <t xml:space="preserve">Vinisha Gladys Belshi </t>
   </si>
   <si>
-    <t>/static/images/profile_photos/001/VEC-001-04-092.jpg</t>
+    <t>/static/images/profile_photos/001/VEC-001-04-092.webp</t>
   </si>
   <si>
     <t>https://scholar.google.com/citations?view_op=new_articles&amp;hl=en&amp;imq=Vinisha+Leo#</t>
@@ -199,7 +199,7 @@
     <t>MYTHILI</t>
   </si>
   <si>
-    <t>/static/images/profile_photos/001/VEC-001-04-087.jpg</t>
+    <t>/static/images/profile_photos/001/VEC-001-04-087.webp</t>
   </si>
   <si>
     <t>nil</t>
@@ -214,7 +214,7 @@
     <t>PRIYA</t>
   </si>
   <si>
-    <t>/static/images/profile_photos/001/VEC-001-04-095.jpg</t>
+    <t>/static/images/profile_photos/001/VEC-001-04-095.webp</t>
   </si>
   <si>
     <t>https://scholar.google.com/citations?view_op=new_articles&amp;hl=en&amp;imq=Priya+Manoharan&amp;authuser=2#</t>
@@ -229,7 +229,7 @@
     <t xml:space="preserve">SAVIJA </t>
   </si>
   <si>
-    <t>/static/images/profile_photos/001/VEC-001-04-074.jpg</t>
+    <t>/static/images/profile_photos/001/VEC-001-04-074.webp</t>
   </si>
   <si>
     <t>https://scholar.google.com/citations?user=mlPrXHcAAAAJ&amp;hl=en</t>
@@ -253,7 +253,7 @@
     <t>SATHISH</t>
   </si>
   <si>
-    <t>/static/images/profile_photos/001/VEC-001-04-056.jpg</t>
+    <t>/static/images/profile_photos/001/VEC-001-04-056.webp</t>
   </si>
   <si>
     <t>https://scholar.google.com/citations?user=fS-k-YYAAAAJ&amp;hl=en</t>
@@ -271,7 +271,7 @@
     <t xml:space="preserve">DEEPA </t>
   </si>
   <si>
-    <t>/static/images/profile_photos/001/VEC-001-04-063.jpg</t>
+    <t>/static/images/profile_photos/001/VEC-001-04-063.webp</t>
   </si>
   <si>
     <t>https://scholar.google.com/citations?hl=en&amp;user=VTfr5bIAAAAJ&amp;authuser=1&amp;scilu=&amp;scisig=AJY4_hMAAAAAZvJL0N4c2ABv_DJa003kQS27dYw&amp;gmla=ALUCkoWakzMFfuzGLaf1xz8mz1PSRXIDTiGHkgbV5L71ewOjRS4U2MlMdeR6VVhI6MUNnCouYeLo6pS_FYSpY6EcwX9ooixn-X1bAKsg4tg&amp;sciund=1483249734394795239</t>
@@ -286,7 +286,7 @@
     <t xml:space="preserve">KARTHIKA </t>
   </si>
   <si>
-    <t>/static/images/profile_photos/001/VEC-001-04-068.jpg</t>
+    <t>/static/images/profile_photos/001/VEC-001-04-068.webp</t>
   </si>
   <si>
     <t xml:space="preserve">https://scholar.google.com/citations?user=_LCpHnMAAAAJ&amp;hl=en </t>
@@ -304,7 +304,7 @@
     <t>Joncy</t>
   </si>
   <si>
-    <t>/static/images/profile_photos/001/VEC-001-04-055.jpg</t>
+    <t>/static/images/profile_photos/001/VEC-001-04-055.webp</t>
   </si>
   <si>
     <t>https://scholar.google.com/citations?hl=en&amp;view_op=list_works&amp;gmla=ALUCkoX59rXtYYTW-pyMab60KZdjFvgcXSeLOiSqucU9wcc_1pTvrsVq3LLR0cJAITVdLwjbgEoWn0vr6cjmqg&amp;user=nUes5HIAAAAJ</t>
@@ -319,7 +319,7 @@
     <t>MIZPAH QUEENY</t>
   </si>
   <si>
-    <t>/static/images/profile_photos/001/VEC-001-04-059.jpg</t>
+    <t>/static/images/profile_photos/001/VEC-001-04-059.webp</t>
   </si>
   <si>
     <t>https://scholar.google.com/citations?hl=en&amp;user=IWH6UaoAAAAJ&amp;authuser=1&amp;scilu=&amp;scisig=AJY4_hMAAAAAZvJNDfT7SquQ5ll7Gwon0oBKDtg&amp;gmla=ALUCkoU_Y0lPdVx69YEjZQXXaU7IrCT033Plba_qewMSa3kYUkqMEcQ5Tqu6F3pbrf2Lnn5yaqEN52oWp2RE5l_D9pR0_3Ni6P9wXdRUIW8&amp;sciund=3769189586746942793</t>
@@ -334,7 +334,7 @@
     <t>Swetha R</t>
   </si>
   <si>
-    <t>/static/images/profile_photos/001/VEC-001-04-094.jpg</t>
+    <t>/static/images/profile_photos/001/VEC-001-04-094.webp</t>
   </si>
   <si>
     <t>https://scholar.google.com/citations?hl=en&amp;user=Cos-0isAAAAJ&amp;scilu=&amp;scisig=AJY4_hMAAAAAZvTt6zb0U8w65xkPiXa95kTvAnU&amp;gmla=ALUCkoW-7v09YTuOhfGWI_gIjagS6iuEs4VOdqS9wA_Pp8kkLcvUZZDt4qOEGqCr_C1kfjXpPseuxeiv-wTlwWoLseavVzt_eqoI_Qj5ChnX&amp;sciund=4015425886573017390</t>
@@ -349,7 +349,7 @@
     <t xml:space="preserve">Manimegalai </t>
   </si>
   <si>
-    <t>/static/images/profile_photos/001/VEC-001-04-067.jpg</t>
+    <t>/static/images/profile_photos/001/VEC-001-04-067.webp</t>
   </si>
   <si>
     <t>https://scholar.google.com/citations?hl=en&amp;user=ql7Q-w4AAAAJ&amp;view_op=list_works&amp;gmla=ALUCkoVZ-qAuRamMDz1bla6tmvYXSzMAgleesdeoGqDbt4SQgKDd2_mEkLjyTOrtnkSCJka5eQGpFaTx2MxL2jUiuDrDaQqjAY6khBU0XmZAunkhQsHmu58jMlKeGqnt_Z4UxTQB9Ckd</t>
@@ -377,7 +377,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -737,8 +737,8 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="32.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="59.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="20.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="50.14785714285715" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>

</xml_diff>

<commit_message>
updated  top nav bar , excel and other jsons
</commit_message>
<xml_diff>
--- a/docs/STAFF-DATA/001.xlsx
+++ b/docs/STAFF-DATA/001.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Velammal-Engineering-College-Backend\docs\STAFF-DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Velammal-Engineering-College-Backend\docs\STAFF-DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E0BA60-DE23-4AC6-872D-65E0CB049240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="116">
   <si>
     <t>Name</t>
   </si>
@@ -308,9 +307,6 @@
   </si>
   <si>
     <t>VEC-001-04-056</t>
-  </si>
-  <si>
-    <t>PRAISEWIN C</t>
   </si>
   <si>
     <t>RAJASUGANYA P V</t>
@@ -376,7 +372,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -735,14 +731,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -790,10 +786,10 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -819,13 +815,13 @@
     </row>
     <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D3" t="s">
         <v>18</v>
@@ -851,10 +847,10 @@
         <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D4" t="s">
         <v>25</v>
@@ -880,10 +876,10 @@
         <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D5" t="s">
         <v>31</v>
@@ -912,10 +908,10 @@
         <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D6" t="s">
         <v>39</v>
@@ -944,10 +940,10 @@
         <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D7" t="s">
         <v>43</v>
@@ -970,10 +966,10 @@
         <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D8" t="s">
         <v>48</v>
@@ -990,10 +986,10 @@
         <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D9" t="s">
         <v>52</v>
@@ -1010,10 +1006,10 @@
         <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D10" t="s">
         <v>56</v>
@@ -1030,10 +1026,10 @@
         <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D11" t="s">
         <v>60</v>
@@ -1059,10 +1055,10 @@
         <v>66</v>
       </c>
       <c r="B12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D12" t="s">
         <v>67</v>
@@ -1085,10 +1081,10 @@
         <v>71</v>
       </c>
       <c r="B13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D13" t="s">
         <v>72</v>
@@ -1105,10 +1101,10 @@
         <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D14" t="s">
         <v>76</v>
@@ -1128,10 +1124,10 @@
         <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D15" t="s">
         <v>80</v>
@@ -1148,10 +1144,10 @@
         <v>83</v>
       </c>
       <c r="B16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D16" t="s">
         <v>84</v>
@@ -1168,10 +1164,10 @@
         <v>87</v>
       </c>
       <c r="B17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D17" t="s">
         <v>88</v>
@@ -1188,10 +1184,10 @@
         <v>91</v>
       </c>
       <c r="B18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D18" t="s">
         <v>92</v>
@@ -1216,33 +1212,13 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>96</v>
-      </c>
-      <c r="B19" t="s">
-        <v>99</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Some Endpoint, Insertion and json are Added
</commit_message>
<xml_diff>
--- a/docs/STAFF-DATA/001.xlsx
+++ b/docs/STAFF-DATA/001.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Velammal-Engineering-College-Backend\docs\STAFF-DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542510BB-F718-48C2-AC47-3EE67D1898AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C47F98-A0A6-453E-ABE6-55B6DEA5A9CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="120">
   <si>
     <t>Name</t>
   </si>
@@ -370,46 +370,16 @@
     <t>/static/images/profile_photos/001/VEC-001-04-056.webp</t>
   </si>
   <si>
-    <t>RASHMI P</t>
-  </si>
-  <si>
-    <t>TAMIL SELVI V</t>
-  </si>
-  <si>
-    <t>JARIYA BEGUM A R</t>
-  </si>
-  <si>
-    <t>RAMYA P</t>
-  </si>
-  <si>
-    <t>/static/images/profile_photos/001/VEC-001-04-621.webp</t>
-  </si>
-  <si>
-    <t>/static/images/profile_photos/001/VEC-001-04-622.webp</t>
-  </si>
-  <si>
-    <t>/static/images/profile_photos/001/VEC-001-04-623.webp</t>
-  </si>
-  <si>
-    <t>/static/images/profile_photos/001/VEC-001-04-624.webp</t>
-  </si>
-  <si>
-    <t>VEC-001-04-621</t>
-  </si>
-  <si>
-    <t>VEC-001-04-622</t>
-  </si>
-  <si>
-    <t>VEC-001-04-623</t>
-  </si>
-  <si>
-    <t>VEC-001-04-624</t>
-  </si>
-  <si>
-    <t>VEC-001-04-625</t>
-  </si>
-  <si>
-    <t>/static/images/profile_photos/001/VEC-001-04-625.webp</t>
+    <t>THAMARAI SELVAN P</t>
+  </si>
+  <si>
+    <t>/static/images/profile_photos/001/VEC-001-05-1.webp</t>
+  </si>
+  <si>
+    <t>VEC-001-05-1</t>
+  </si>
+  <si>
+    <t>Lab Instructor</t>
   </si>
 </sst>
 </file>
@@ -482,13 +452,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -795,17 +764,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.77734375" customWidth="1"/>
+    <col min="3" max="3" width="50.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1272,14 +1241,14 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>116</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
+      </c>
+      <c r="C19" t="s">
+        <v>117</v>
       </c>
       <c r="D19" s="2"/>
       <c r="F19" s="2"/>
@@ -1287,63 +1256,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="J20" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
         <v>118</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="J21" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="J22" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="J23" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added institutional distinctiveness in IQAC
</commit_message>
<xml_diff>
--- a/docs/STAFF-DATA/001.xlsx
+++ b/docs/STAFF-DATA/001.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Velammal-Engineering-College-Backend\docs\STAFF-DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepa\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542510BB-F718-48C2-AC47-3EE67D1898AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1EABCDC3-7FC3-4E5F-8F4A-9800A04E2A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="134">
   <si>
     <t>Name</t>
   </si>
@@ -370,46 +370,58 @@
     <t>/static/images/profile_photos/001/VEC-001-04-056.webp</t>
   </si>
   <si>
+    <t>THAMARAI SELVAN P</t>
+  </si>
+  <si>
+    <t>/static/images/profile_photos/001/VEC-001-05-1.webp</t>
+  </si>
+  <si>
+    <t>VEC-001-05-1</t>
+  </si>
+  <si>
+    <t>Lab Instructor</t>
+  </si>
+  <si>
     <t>RASHMI P</t>
   </si>
   <si>
+    <t>/static/images/profile_photos/001/VEC-001-04-621.webp</t>
+  </si>
+  <si>
+    <t>VEC-001-04-621</t>
+  </si>
+  <si>
     <t>TAMIL SELVI V</t>
   </si>
   <si>
+    <t>/static/images/profile_photos/001/VEC-001-04-622.webp</t>
+  </si>
+  <si>
+    <t>VEC-001-04-622</t>
+  </si>
+  <si>
     <t>JARIYA BEGUM A R</t>
   </si>
   <si>
+    <t>/static/images/profile_photos/001/VEC-001-04-623.webp</t>
+  </si>
+  <si>
+    <t>VEC-001-04-623</t>
+  </si>
+  <si>
+    <t>/static/images/profile_photos/001/VEC-001-04-624.webp</t>
+  </si>
+  <si>
+    <t>VEC-001-04-624</t>
+  </si>
+  <si>
     <t>RAMYA P</t>
   </si>
   <si>
-    <t>/static/images/profile_photos/001/VEC-001-04-621.webp</t>
-  </si>
-  <si>
-    <t>/static/images/profile_photos/001/VEC-001-04-622.webp</t>
-  </si>
-  <si>
-    <t>/static/images/profile_photos/001/VEC-001-04-623.webp</t>
-  </si>
-  <si>
-    <t>/static/images/profile_photos/001/VEC-001-04-624.webp</t>
-  </si>
-  <si>
-    <t>VEC-001-04-621</t>
-  </si>
-  <si>
-    <t>VEC-001-04-622</t>
-  </si>
-  <si>
-    <t>VEC-001-04-623</t>
-  </si>
-  <si>
-    <t>VEC-001-04-624</t>
+    <t>/static/images/profile_photos/001/VEC-001-04-625.webp</t>
   </si>
   <si>
     <t>VEC-001-04-625</t>
-  </si>
-  <si>
-    <t>/static/images/profile_photos/001/VEC-001-04-625.webp</t>
   </si>
 </sst>
 </file>
@@ -482,13 +494,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -795,17 +806,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.77734375" customWidth="1"/>
+    <col min="3" max="3" width="50.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1271,15 +1282,15 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C19" s="3" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
         <v>120</v>
+      </c>
+      <c r="B19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" t="s">
+        <v>121</v>
       </c>
       <c r="D19" s="2"/>
       <c r="F19" s="2"/>
@@ -1287,63 +1298,82 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>121</v>
       </c>
       <c r="J20" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B21" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" t="s">
+        <v>127</v>
+      </c>
+      <c r="J21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" t="s">
+        <v>129</v>
+      </c>
+      <c r="J22" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B23" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" t="s">
+        <v>132</v>
+      </c>
+      <c r="J23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" t="s">
+        <v>117</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="J21" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="J22" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="J23" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
library , IQAC , Staff excel are updated
</commit_message>
<xml_diff>
--- a/docs/STAFF-DATA/001.xlsx
+++ b/docs/STAFF-DATA/001.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Velammal-Engineering-College-Backend\docs\STAFF-DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Velammal-Engineering-College-Backend\docs\STAFF-DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D77495-A5A5-478C-887A-AECD7FEC6748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6228"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,12 +82,21 @@
     <t>VEC-001-01-077</t>
   </si>
   <si>
-    <t>RAJASUGANYA P V</t>
-  </si>
-  <si>
     <t>Assistant Professor</t>
   </si>
   <si>
+    <t>/static/images/profile_photos/001/VEC-001-04-080.webp</t>
+  </si>
+  <si>
+    <t>https://scholar.google.co.in/citations?view_op=new_articles&amp;hl=en&amp;imq=prema%40velammal.edu.in&amp;nuan-1=premanila21%40gmail.com&amp;authuser=1#</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/prema-amirthalingam-10b3726a/</t>
+  </si>
+  <si>
+    <t>VEC-001-04-080</t>
+  </si>
+  <si>
     <t>/static/images/profile_photos/001/VEC-001-04-085.webp</t>
   </si>
   <si>
@@ -108,9 +118,6 @@
     <t>VEC-001-04-085</t>
   </si>
   <si>
-    <t>KAVITHA R</t>
-  </si>
-  <si>
     <t>/static/images/profile_photos/001/VEC-001-04-075.webp</t>
   </si>
   <si>
@@ -126,9 +133,6 @@
     <t>VEC-001-04-075</t>
   </si>
   <si>
-    <t>HANNAH ROSE ESTHER T</t>
-  </si>
-  <si>
     <t>/static/images/profile_photos/001/VEC-001-04-060.webp</t>
   </si>
   <si>
@@ -153,24 +157,6 @@
     <t>VEC-001-04-060</t>
   </si>
   <si>
-    <t>PREMA A</t>
-  </si>
-  <si>
-    <t>/static/images/profile_photos/001/VEC-001-04-080.webp</t>
-  </si>
-  <si>
-    <t>https://scholar.google.co.in/citations?view_op=new_articles&amp;hl=en&amp;imq=prema%40velammal.edu.in&amp;nuan-1=premanila21%40gmail.com&amp;authuser=1#</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/prema-amirthalingam-10b3726a/</t>
-  </si>
-  <si>
-    <t>VEC-001-04-080</t>
-  </si>
-  <si>
-    <t>VIJAYALAKSHMI S</t>
-  </si>
-  <si>
     <t>/static/images/profile_photos/001/VEC-001-04-086.webp</t>
   </si>
   <si>
@@ -186,9 +172,6 @@
     <t>VEC-001-04-086</t>
   </si>
   <si>
-    <t>MYTHILI S</t>
-  </si>
-  <si>
     <t>/static/images/profile_photos/001/VEC-001-04-087.webp</t>
   </si>
   <si>
@@ -201,9 +184,6 @@
     <t>VEC-001-04-087</t>
   </si>
   <si>
-    <t>PRIYA M</t>
-  </si>
-  <si>
     <t>/static/images/profile_photos/001/VEC-001-04-095.webp</t>
   </si>
   <si>
@@ -216,9 +196,6 @@
     <t>VEC-001-04-095</t>
   </si>
   <si>
-    <t>KARTHIKA L</t>
-  </si>
-  <si>
     <t>/static/images/profile_photos/001/VEC-001-04-068.webp</t>
   </si>
   <si>
@@ -234,9 +211,6 @@
     <t>VEC-001-04-068</t>
   </si>
   <si>
-    <t>JONCY J</t>
-  </si>
-  <si>
     <t>/static/images/profile_photos/001/VEC-001-04-055.webp</t>
   </si>
   <si>
@@ -249,9 +223,6 @@
     <t>VEC-001-04-055</t>
   </si>
   <si>
-    <t>MANIMEGALAI L</t>
-  </si>
-  <si>
     <t>/static/images/profile_photos/001/VEC-001-04-067.webp</t>
   </si>
   <si>
@@ -264,9 +235,6 @@
     <t>VEC-001-04-067</t>
   </si>
   <si>
-    <t>DEEPA S</t>
-  </si>
-  <si>
     <t>/static/images/profile_photos/001/VEC-001-04-063.webp</t>
   </si>
   <si>
@@ -279,9 +247,6 @@
     <t>VEC-001-04-063</t>
   </si>
   <si>
-    <t>MIZPAH QUEENY R</t>
-  </si>
-  <si>
     <t>/static/images/profile_photos/001/VEC-001-04-059.webp</t>
   </si>
   <si>
@@ -294,9 +259,6 @@
     <t>VEC-001-04-059</t>
   </si>
   <si>
-    <t>SWETHA R</t>
-  </si>
-  <si>
     <t>/static/images/profile_photos/001/VEC-001-04-094.webp</t>
   </si>
   <si>
@@ -309,9 +271,6 @@
     <t>VEC-001-04-094</t>
   </si>
   <si>
-    <t>SATHISH K</t>
-  </si>
-  <si>
     <t>/static/images/profile_photos/001/VEC-001-04-056.webp</t>
   </si>
   <si>
@@ -327,27 +286,18 @@
     <t>VEC-001-04-056</t>
   </si>
   <si>
-    <t>RASHMI P</t>
-  </si>
-  <si>
     <t>/static/images/profile_photos/001/VEC-001-04-621.webp</t>
   </si>
   <si>
     <t>VEC-001-04-621</t>
   </si>
   <si>
-    <t>TAMIL SELVI V</t>
-  </si>
-  <si>
     <t>/static/images/profile_photos/001/VEC-001-04-622.webp</t>
   </si>
   <si>
     <t>VEC-001-04-622</t>
   </si>
   <si>
-    <t>JARIYA BEGUM A R</t>
-  </si>
-  <si>
     <t>/static/images/profile_photos/001/VEC-001-04-623.webp</t>
   </si>
   <si>
@@ -360,18 +310,12 @@
     <t>VEC-001-04-624</t>
   </si>
   <si>
-    <t>RAMYA P</t>
-  </si>
-  <si>
     <t>/static/images/profile_photos/001/VEC-001-04-625.webp</t>
   </si>
   <si>
     <t>VEC-001-04-625</t>
   </si>
   <si>
-    <t>THAMARAI SELVAN P</t>
-  </si>
-  <si>
     <t>Lab Instructor</t>
   </si>
   <si>
@@ -379,12 +323,69 @@
   </si>
   <si>
     <t>VEC-001-05-001</t>
+  </si>
+  <si>
+    <t>Mrs. RAJASUGANYA P V</t>
+  </si>
+  <si>
+    <t>Mrs. KAVITHA R</t>
+  </si>
+  <si>
+    <t>Mrs. HANNAH ROSE ESTHER T</t>
+  </si>
+  <si>
+    <t>Mrs. VIJAYALAKSHMI S</t>
+  </si>
+  <si>
+    <t>Mrs. MYTHILI S</t>
+  </si>
+  <si>
+    <t>Mrs. PRIYA M</t>
+  </si>
+  <si>
+    <t>Mrs. KARTHIKA L</t>
+  </si>
+  <si>
+    <t>Mrs. JONCY J</t>
+  </si>
+  <si>
+    <t>Mrs. MANIMEGALAI L</t>
+  </si>
+  <si>
+    <t>Mrs. DEEPA S</t>
+  </si>
+  <si>
+    <t>Mrs. MIZPAH QUEENY R</t>
+  </si>
+  <si>
+    <t>Mrs. SWETHA R</t>
+  </si>
+  <si>
+    <t>Mr. SATHISH K</t>
+  </si>
+  <si>
+    <t>Mrs. RASHMI P</t>
+  </si>
+  <si>
+    <t>Mrs. TAMIL SELVI V</t>
+  </si>
+  <si>
+    <t>Mrs. JARIYA BEGUM A R</t>
+  </si>
+  <si>
+    <t>Mrs. RAMYA P</t>
+  </si>
+  <si>
+    <t>Mrs. PREMA A</t>
+  </si>
+  <si>
+    <t>Mr. THAMARAI SELVAN P</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -402,7 +403,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -442,16 +443,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -753,22 +755,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="10" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -810,509 +812,429 @@
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>44</v>
+        <v>118</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>48</v>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="D4" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="F4" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="G4" t="s">
         <v>28</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
         <v>32</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="D5" t="s">
         <v>33</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="H5" t="s">
         <v>34</v>
+      </c>
+      <c r="I5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>35</v>
+        <v>103</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="D6" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="E6" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="F6" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="G6" t="s">
         <v>41</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="H6" t="s">
         <v>42</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="I6" t="s">
         <v>43</v>
+      </c>
+      <c r="J6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" t="s">
         <v>49</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>59</v>
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" t="s">
+        <v>52</v>
+      </c>
+      <c r="J8" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>60</v>
+        <v>106</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>64</v>
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" t="s">
+        <v>56</v>
+      </c>
+      <c r="J9" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>65</v>
+        <v>107</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>70</v>
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>71</v>
+        <v>108</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>75</v>
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" t="s">
+        <v>64</v>
+      </c>
+      <c r="I11" t="s">
+        <v>65</v>
+      </c>
+      <c r="J11" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>76</v>
+        <v>109</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>80</v>
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" t="s">
+        <v>68</v>
+      </c>
+      <c r="I12" t="s">
+        <v>69</v>
+      </c>
+      <c r="J12" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>85</v>
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" t="s">
+        <v>72</v>
+      </c>
+      <c r="I13" t="s">
+        <v>73</v>
+      </c>
+      <c r="J13" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>90</v>
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" t="s">
+        <v>76</v>
+      </c>
+      <c r="I14" t="s">
+        <v>77</v>
+      </c>
+      <c r="J14" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>95</v>
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" t="s">
+        <v>80</v>
+      </c>
+      <c r="I15" t="s">
+        <v>81</v>
+      </c>
+      <c r="J15" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>101</v>
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16" t="s">
+        <v>85</v>
+      </c>
+      <c r="I16" t="s">
+        <v>86</v>
+      </c>
+      <c r="J16" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2" t="s">
-        <v>104</v>
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>88</v>
+      </c>
+      <c r="J17" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2" t="s">
-        <v>107</v>
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>90</v>
+      </c>
+      <c r="J18" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2" t="s">
-        <v>110</v>
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>92</v>
+      </c>
+      <c r="J19" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2" t="s">
-        <v>112</v>
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
+        <v>94</v>
+      </c>
+      <c r="J20" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2" t="s">
-        <v>115</v>
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>96</v>
+      </c>
+      <c r="J21" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2" t="s">
-        <v>119</v>
+        <v>98</v>
+      </c>
+      <c r="C22" t="s">
+        <v>99</v>
+      </c>
+      <c r="J22" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>